<commit_message>
adding modified related resources
</commit_message>
<xml_diff>
--- a/test-data/related-resources-data.xlsx
+++ b/test-data/related-resources-data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11209"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/learnb/git/digiplat-qa/test-data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/geopopkh/eclipse-workspace/cgov-digital-platform-qa/test-data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02BCA1F6-F25B-0B49-99A0-897D902012A7}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A78AA75-61D6-4F40-B186-7BAE5658ED4E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="23560" yWindow="4400" windowWidth="27640" windowHeight="16940" activeTab="1" xr2:uid="{112BCE41-1B7B-AF44-BEF2-07A92CFC037C}"/>
+    <workbookView xWindow="1160" yWindow="460" windowWidth="27640" windowHeight="15940" xr2:uid="{112BCE41-1B7B-AF44-BEF2-07A92CFC037C}"/>
   </bookViews>
   <sheets>
     <sheet name="pages_with_related_resources" sheetId="1" r:id="rId1"/>
@@ -21,17 +21,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="9">
   <si>
     <t>path</t>
   </si>
@@ -52,6 +47,12 @@
   </si>
   <si>
     <t>node/21</t>
+  </si>
+  <si>
+    <t>about-nci/organization/sharpless-nci-director</t>
+  </si>
+  <si>
+    <t>Press Release</t>
   </si>
 </sst>
 </file>
@@ -403,10 +404,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6ABDEF67-3BF3-604C-97A8-A43819B8E79D}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:C2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -437,6 +438,17 @@
         <v>5</v>
       </c>
     </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -446,7 +458,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E4A3B0B-8B0F-6546-A344-A90113573E35}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
adding modified test data file for Related Resources
</commit_message>
<xml_diff>
--- a/test-data/related-resources-data.xlsx
+++ b/test-data/related-resources-data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/geopopkh/eclipse-workspace/cgov-digital-platform-qa/test-data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A78AA75-61D6-4F40-B186-7BAE5658ED4E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FC49F85-9468-FF45-AD47-5D34AA847E05}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1160" yWindow="460" windowWidth="27640" windowHeight="15940" xr2:uid="{112BCE41-1B7B-AF44-BEF2-07A92CFC037C}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15940" xr2:uid="{112BCE41-1B7B-AF44-BEF2-07A92CFC037C}"/>
   </bookViews>
   <sheets>
     <sheet name="pages_with_related_resources" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="16">
   <si>
     <t>path</t>
   </si>
@@ -46,13 +46,34 @@
     <t>English</t>
   </si>
   <si>
-    <t>node/21</t>
-  </si>
-  <si>
-    <t>about-nci/organization/sharpless-nci-director</t>
+    <t>Spanish</t>
+  </si>
+  <si>
+    <t>Blog</t>
+  </si>
+  <si>
+    <t>espanol/cancer/sobrellevar/sentimientos/hoja-informativa-estres</t>
   </si>
   <si>
     <t>Press Release</t>
+  </si>
+  <si>
+    <t>sharpless-nci-director</t>
+  </si>
+  <si>
+    <t>about-cancer/coping/feelings/relaxation/vitamin-d-supplement-cancer-prevention</t>
+  </si>
+  <si>
+    <t>Blog Page</t>
+  </si>
+  <si>
+    <t>news-events/press-releases/2018/oropharyngeal-hpv-cisplatin</t>
+  </si>
+  <si>
+    <t>espanol/about-cancer/coping/feelings/relaxation/vitamina-d-complemento-cancer-prevencion</t>
+  </si>
+  <si>
+    <t>news-events/cancer-currents-blog/2019/human-tumor-atlas-network-cancer-maps</t>
   </si>
 </sst>
 </file>
@@ -88,8 +109,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -404,16 +429,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6ABDEF67-3BF3-604C-97A8-A43819B8E79D}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="36.83203125" customWidth="1"/>
-    <col min="2" max="2" width="13.33203125" customWidth="1"/>
+    <col min="1" max="1" width="74.6640625" customWidth="1"/>
+    <col min="2" max="2" width="23.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
@@ -427,8 +452,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+    <row r="2" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B2" t="s">
@@ -440,12 +465,34 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" t="s">
         <v>5</v>
       </c>
     </row>
@@ -456,13 +503,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E4A3B0B-8B0F-6546-A344-A90113573E35}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="94.6640625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -477,12 +527,34 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B2" t="s">
         <v>4</v>
       </c>
       <c r="C2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>